<commit_message>
- actualizar path reproducible
</commit_message>
<xml_diff>
--- a/datos_audio.xlsx
+++ b/datos_audio.xlsx
@@ -86,37 +86,37 @@
     <t>Dios, en el principio, creó los cielos y la tierra.</t>
   </si>
   <si>
-    <t>RepositorioDatosProyectoAP/AudiosReproducible/biblia.wav</t>
+    <t>RepositorioDatosProyectoAP/AudiosReproducibles/biblia.wav</t>
   </si>
   <si>
     <t>Calisto arde en amores de Melibea. De ti y de mí tiene necesidad.</t>
   </si>
   <si>
-    <t>RepositorioDatosProyectoAP/AudiosReproducible/celestina.wav</t>
+    <t>RepositorioDatosProyectoAP/AudiosReproducibles/celestina.wav</t>
   </si>
   <si>
     <t>Señoras y señores, muchas tardes y buenas gracias.</t>
   </si>
   <si>
-    <t>RepositorioDatosProyectoAP/AudiosReproducible/m.rajoy.wav</t>
+    <t>RepositorioDatosProyectoAP/AudiosReproducibles/m.rajoy.wav</t>
   </si>
   <si>
     <t>Érase una vez un anciano carpintero llamado Gepeto.</t>
   </si>
   <si>
-    <t>RepositorioDatosProyectoAP/AudiosReproducible/pinocho.wav</t>
+    <t>RepositorioDatosProyectoAP/AudiosReproducibles/pinocho.wav</t>
   </si>
   <si>
     <t>Las serpientes boas tragan a su presa entera</t>
   </si>
   <si>
-    <t>RepositorioDatosProyectoAP/AudiosReproducible/principito.wav</t>
+    <t>RepositorioDatosProyectoAP/AudiosReproducibles/principito.wav</t>
   </si>
   <si>
     <t>La recta de mínimos cuadrados es la que minimiza la distancia de mínimos cuadrados.</t>
   </si>
   <si>
-    <t>RepositorioDatosProyectoAP/AudiosReproducible/recta_mc.wav</t>
+    <t>RepositorioDatosProyectoAP/AudiosReproducibles/recta_mc.wav</t>
   </si>
 </sst>
 </file>

</xml_diff>